<commit_message>
regret experiment done, and FAA files are now complete, with new reward structure
</commit_message>
<xml_diff>
--- a/stationarity_test/KLDivergenceTest/FeedbackLog/p10-faa-0ms.xlsx
+++ b/stationarity_test/KLDivergenceTest/FeedbackLog/p10-faa-0ms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanadsaha92/Desktop/Research_Experiments/imMens-Interactions/stationarity_test/KLDivergenceTest/FeedbackLog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7CEE35-D0C3-CA44-AAE5-CCF74E45CD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5393B6-563D-5147-913D-746DDD9E972D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="161">
   <si>
     <t>proposition</t>
   </si>
@@ -537,11 +537,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4939,7 +4941,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9440,10 +9442,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:G998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9485,7 +9487,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>156</v>
@@ -9508,7 +9510,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>156</v>
@@ -9528,56 +9530,56 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4">
-        <v>1.1574074074074264E-4</v>
+        <v>2.7777777777777957E-4</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="4">
-        <v>1.6203703703703692E-4</v>
+        <v>4.2824074074074292E-4</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -9589,7 +9591,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="4">
-        <v>2.7777777777777957E-4</v>
+        <v>5.0925925925926138E-4</v>
       </c>
       <c r="G6" s="2">
         <v>2</v>
@@ -9597,10 +9599,10 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -9612,7 +9614,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="4">
-        <v>4.2824074074074292E-4</v>
+        <v>5.2083333333333495E-4</v>
       </c>
       <c r="G7" s="2">
         <v>2</v>
@@ -9620,10 +9622,10 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -9635,7 +9637,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="4">
-        <v>5.0925925925926138E-4</v>
+        <v>8.6805555555555594E-4</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
@@ -9643,10 +9645,10 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -9658,7 +9660,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="4">
-        <v>5.2083333333333495E-4</v>
+        <v>1.0995370370370378E-3</v>
       </c>
       <c r="G9" s="2">
         <v>2</v>
@@ -9666,10 +9668,10 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -9681,7 +9683,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="4">
-        <v>8.6805555555555594E-4</v>
+        <v>1.1342592592592585E-3</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
@@ -9689,10 +9691,10 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -9704,7 +9706,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="4">
-        <v>1.0995370370370378E-3</v>
+        <v>1.1921296296296298E-3</v>
       </c>
       <c r="G11" s="2">
         <v>2</v>
@@ -9712,10 +9714,10 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -9727,7 +9729,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="4">
-        <v>1.1342592592592585E-3</v>
+        <v>1.2500000000000011E-3</v>
       </c>
       <c r="G12" s="2">
         <v>2</v>
@@ -9735,22 +9737,22 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="4">
-        <v>1.1921296296296298E-3</v>
+        <v>1.2615740740740747E-3</v>
       </c>
       <c r="G13" s="2">
         <v>2</v>
@@ -9758,10 +9760,10 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
@@ -9773,7 +9775,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="4">
-        <v>1.2500000000000011E-3</v>
+        <v>1.3425925925925931E-3</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
@@ -9781,22 +9783,22 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="4">
-        <v>1.2615740740740747E-3</v>
+        <v>1.3657407407407403E-3</v>
       </c>
       <c r="G15" s="2">
         <v>2</v>
@@ -9804,22 +9806,22 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="4">
-        <v>1.3425925925925931E-3</v>
+        <v>1.4004629629629645E-3</v>
       </c>
       <c r="G16" s="2">
         <v>2</v>
@@ -9827,22 +9829,22 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4">
-        <v>1.3657407407407403E-3</v>
+        <v>1.5277777777777772E-3</v>
       </c>
       <c r="G17" s="2">
         <v>2</v>
@@ -9850,13 +9852,13 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>32</v>
@@ -9865,7 +9867,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="4">
-        <v>1.4004629629629645E-3</v>
+        <v>1.5972222222222221E-3</v>
       </c>
       <c r="G18" s="2">
         <v>2</v>
@@ -9873,22 +9875,22 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="4">
-        <v>1.5277777777777772E-3</v>
+        <v>1.6782407407407406E-3</v>
       </c>
       <c r="G19" s="2">
         <v>2</v>
@@ -9896,22 +9898,22 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20" s="4">
-        <v>1.5972222222222221E-3</v>
+        <v>1.7361111111111119E-3</v>
       </c>
       <c r="G20" s="2">
         <v>2</v>
@@ -9919,22 +9921,22 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="4">
-        <v>1.6782407407407406E-3</v>
+        <v>1.8055555555555568E-3</v>
       </c>
       <c r="G21" s="2">
         <v>2</v>
@@ -9942,10 +9944,10 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
@@ -9957,7 +9959,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="4">
-        <v>1.7361111111111119E-3</v>
+        <v>1.8634259259259281E-3</v>
       </c>
       <c r="G22" s="2">
         <v>2</v>
@@ -9965,10 +9967,10 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
@@ -9980,7 +9982,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="4">
-        <v>1.8055555555555568E-3</v>
+        <v>1.8981481481481488E-3</v>
       </c>
       <c r="G23" s="2">
         <v>2</v>
@@ -9988,10 +9990,10 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>17</v>
@@ -10003,7 +10005,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="4">
-        <v>1.8634259259259281E-3</v>
+        <v>1.9791666666666673E-3</v>
       </c>
       <c r="G24" s="2">
         <v>2</v>
@@ -10011,10 +10013,10 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
@@ -10026,7 +10028,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="4">
-        <v>1.8981481481481488E-3</v>
+        <v>2.0370370370370386E-3</v>
       </c>
       <c r="G25" s="2">
         <v>2</v>
@@ -10034,10 +10036,10 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
@@ -10049,7 +10051,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="4">
-        <v>1.9791666666666673E-3</v>
+        <v>2.0717592592592593E-3</v>
       </c>
       <c r="G26" s="2">
         <v>2</v>
@@ -10057,22 +10059,22 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
       </c>
       <c r="F27" s="4">
-        <v>2.0370370370370386E-3</v>
+        <v>2.1296296296296306E-3</v>
       </c>
       <c r="G27" s="2">
         <v>2</v>
@@ -10080,10 +10082,10 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>17</v>
@@ -10095,7 +10097,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="4">
-        <v>2.0717592592592593E-3</v>
+        <v>2.1412037037037042E-3</v>
       </c>
       <c r="G28" s="2">
         <v>2</v>
@@ -10103,22 +10105,22 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
       </c>
       <c r="F29" s="4">
-        <v>2.1296296296296306E-3</v>
+        <v>2.2106481481481491E-3</v>
       </c>
       <c r="G29" s="2">
         <v>2</v>
@@ -10126,10 +10128,10 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>17</v>
@@ -10141,7 +10143,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="4">
-        <v>2.1412037037037042E-3</v>
+        <v>2.2685185185185204E-3</v>
       </c>
       <c r="G30" s="2">
         <v>2</v>
@@ -10149,22 +10151,22 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B31" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E31" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>2.2106481481481491E-3</v>
+        <v>2.3148148148148147E-3</v>
       </c>
       <c r="G31" s="2">
         <v>2</v>
@@ -10172,22 +10174,22 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E32" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F32" s="4">
-        <v>2.2685185185185204E-3</v>
+        <v>2.5000000000000022E-3</v>
       </c>
       <c r="G32" s="2">
         <v>2</v>
@@ -10195,7 +10197,7 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -10204,13 +10206,13 @@
         <v>17</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="4">
-        <v>2.3148148148148147E-3</v>
+        <v>2.5810185185185207E-3</v>
       </c>
       <c r="G33" s="2">
         <v>2</v>
@@ -10218,22 +10220,22 @@
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="4">
-        <v>2.5000000000000022E-3</v>
+        <v>2.719907407407407E-3</v>
       </c>
       <c r="G34" s="2">
         <v>2</v>
@@ -10241,22 +10243,22 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B35" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="4">
-        <v>2.5810185185185207E-3</v>
+        <v>2.8240740740740761E-3</v>
       </c>
       <c r="G35" s="2">
         <v>2</v>
@@ -10264,22 +10266,22 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E36" s="1">
         <v>2</v>
       </c>
       <c r="F36" s="4">
-        <v>2.719907407407407E-3</v>
+        <v>3.0092592592592601E-3</v>
       </c>
       <c r="G36" s="2">
         <v>2</v>
@@ -10287,22 +10289,22 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E37" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" s="4">
-        <v>2.8240740740740761E-3</v>
+        <v>3.078703703703705E-3</v>
       </c>
       <c r="G37" s="2">
         <v>2</v>
@@ -10310,22 +10312,22 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E38" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F38" s="4">
-        <v>3.0092592592592601E-3</v>
+        <v>3.2175925925925948E-3</v>
       </c>
       <c r="G38" s="2">
         <v>2</v>
@@ -10333,68 +10335,68 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B39" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="E39" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39" s="4">
-        <v>3.078703703703705E-3</v>
+        <v>3.333333333333334E-3</v>
       </c>
       <c r="G39" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B40" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" s="4">
-        <v>3.2175925925925948E-3</v>
+        <v>3.6111111111111101E-3</v>
       </c>
       <c r="G40" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B41" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="E41" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" s="4">
-        <v>3.333333333333334E-3</v>
+        <v>3.773148148148147E-3</v>
       </c>
       <c r="G41" s="2">
         <v>3</v>
@@ -10402,22 +10404,22 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B42" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E42" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" s="4">
-        <v>3.6111111111111101E-3</v>
+        <v>3.9004629629629632E-3</v>
       </c>
       <c r="G42" s="2">
         <v>3</v>
@@ -10425,22 +10427,22 @@
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E43" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43" s="4">
-        <v>3.773148148148147E-3</v>
+        <v>4.2245370370370371E-3</v>
       </c>
       <c r="G43" s="2">
         <v>3</v>
@@ -10448,22 +10450,22 @@
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E44" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F44" s="4">
-        <v>3.9004629629629632E-3</v>
+        <v>4.3402777777777797E-3</v>
       </c>
       <c r="G44" s="2">
         <v>3</v>
@@ -10471,10 +10473,10 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B45" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>156</v>
@@ -10486,7 +10488,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="4">
-        <v>4.2245370370370371E-3</v>
+        <v>4.4212962962962982E-3</v>
       </c>
       <c r="G45" s="2">
         <v>3</v>
@@ -10494,22 +10496,22 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>4.3402777777777797E-3</v>
+        <v>4.5833333333333351E-3</v>
       </c>
       <c r="G46" s="2">
         <v>3</v>
@@ -10517,22 +10519,22 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B47" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="4">
-        <v>4.4212962962962982E-3</v>
+        <v>4.6875000000000007E-3</v>
       </c>
       <c r="G47" s="2">
         <v>3</v>
@@ -10540,22 +10542,22 @@
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B48" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E48" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F48" s="4">
-        <v>4.5833333333333351E-3</v>
+        <v>4.9884259259259274E-3</v>
       </c>
       <c r="G48" s="2">
         <v>3</v>
@@ -10563,22 +10565,22 @@
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B49" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E49" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F49" s="4">
-        <v>4.6875000000000007E-3</v>
+        <v>5.2662037037037035E-3</v>
       </c>
       <c r="G49" s="2">
         <v>3</v>
@@ -10586,22 +10588,22 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B50" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E50" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F50" s="4">
-        <v>4.9884259259259274E-3</v>
+        <v>5.3240740740740748E-3</v>
       </c>
       <c r="G50" s="2">
         <v>3</v>
@@ -10609,22 +10611,22 @@
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="4">
-        <v>5.2662037037037035E-3</v>
+        <v>5.613425925925928E-3</v>
       </c>
       <c r="G51" s="2">
         <v>3</v>
@@ -10632,22 +10634,22 @@
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B52" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E52" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F52" s="4">
-        <v>5.3240740740740748E-3</v>
+        <v>5.7523148148148143E-3</v>
       </c>
       <c r="G52" s="2">
         <v>3</v>
@@ -10655,10 +10657,10 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B53" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>17</v>
@@ -10667,10 +10669,10 @@
         <v>18</v>
       </c>
       <c r="E53" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" s="4">
-        <v>5.613425925925928E-3</v>
+        <v>5.7870370370370385E-3</v>
       </c>
       <c r="G53" s="2">
         <v>3</v>
@@ -10678,10 +10680,10 @@
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B54" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>17</v>
@@ -10690,10 +10692,10 @@
         <v>18</v>
       </c>
       <c r="E54" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" s="4">
-        <v>5.7523148148148143E-3</v>
+        <v>5.9490740740740754E-3</v>
       </c>
       <c r="G54" s="2">
         <v>3</v>
@@ -10701,22 +10703,22 @@
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B55" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E55" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F55" s="4">
-        <v>5.7870370370370385E-3</v>
+        <v>6.0648148148148145E-3</v>
       </c>
       <c r="G55" s="2">
         <v>3</v>
@@ -10724,10 +10726,10 @@
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B56" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>17</v>
@@ -10736,10 +10738,10 @@
         <v>18</v>
       </c>
       <c r="E56" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F56" s="4">
-        <v>5.9490740740740754E-3</v>
+        <v>6.1689814814814836E-3</v>
       </c>
       <c r="G56" s="2">
         <v>3</v>
@@ -10747,22 +10749,22 @@
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B57" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E57" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F57" s="4">
-        <v>6.0648148148148145E-3</v>
+        <v>6.3425925925925941E-3</v>
       </c>
       <c r="G57" s="2">
         <v>3</v>
@@ -10770,22 +10772,22 @@
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B58" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E58" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F58" s="4">
-        <v>6.1689814814814836E-3</v>
+        <v>6.4583333333333333E-3</v>
       </c>
       <c r="G58" s="2">
         <v>3</v>
@@ -10793,10 +10795,10 @@
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B59" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>17</v>
@@ -10808,7 +10810,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="4">
-        <v>6.3425925925925941E-3</v>
+        <v>6.5624999999999989E-3</v>
       </c>
       <c r="G59" s="2">
         <v>3</v>
@@ -10816,22 +10818,22 @@
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B60" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E60" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F60" s="4">
-        <v>6.4583333333333333E-3</v>
+        <v>6.6319444444444438E-3</v>
       </c>
       <c r="G60" s="2">
         <v>3</v>
@@ -10839,22 +10841,22 @@
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B61" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E61" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F61" s="4">
-        <v>6.5624999999999989E-3</v>
+        <v>6.7476851851851864E-3</v>
       </c>
       <c r="G61" s="2">
         <v>3</v>
@@ -10862,22 +10864,22 @@
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B62" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
       </c>
       <c r="F62" s="4">
-        <v>6.6319444444444438E-3</v>
+        <v>7.1180555555555546E-3</v>
       </c>
       <c r="G62" s="2">
         <v>3</v>
@@ -10885,22 +10887,22 @@
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E63" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="4">
-        <v>6.7476851851851864E-3</v>
+        <v>7.2453703703703708E-3</v>
       </c>
       <c r="G63" s="2">
         <v>3</v>
@@ -10908,22 +10910,22 @@
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B64" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E64" s="1">
         <v>2</v>
       </c>
       <c r="F64" s="4">
-        <v>7.1180555555555546E-3</v>
+        <v>7.3495370370370364E-3</v>
       </c>
       <c r="G64" s="2">
         <v>3</v>
@@ -10931,22 +10933,22 @@
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B65" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E65" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F65" s="4">
-        <v>7.2453703703703708E-3</v>
+        <v>7.5694444444444446E-3</v>
       </c>
       <c r="G65" s="2">
         <v>3</v>
@@ -10954,10 +10956,10 @@
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B66" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>17</v>
@@ -10969,7 +10971,7 @@
         <v>2</v>
       </c>
       <c r="F66" s="4">
-        <v>7.3495370370370364E-3</v>
+        <v>7.6851851851851873E-3</v>
       </c>
       <c r="G66" s="2">
         <v>3</v>
@@ -10977,22 +10979,22 @@
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E67" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F67" s="4">
-        <v>7.5694444444444446E-3</v>
+        <v>7.8356481481481471E-3</v>
       </c>
       <c r="G67" s="2">
         <v>3</v>
@@ -11000,22 +11002,22 @@
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B68" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E68" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F68" s="4">
-        <v>7.6851851851851873E-3</v>
+        <v>8.0324074074074082E-3</v>
       </c>
       <c r="G68" s="2">
         <v>3</v>
@@ -11023,22 +11025,22 @@
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B69" s="1">
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E69" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F69" s="4">
-        <v>7.8356481481481471E-3</v>
+        <v>8.171296296296298E-3</v>
       </c>
       <c r="G69" s="2">
         <v>3</v>
@@ -11046,22 +11048,22 @@
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B70" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E70" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F70" s="4">
-        <v>8.0324074074074082E-3</v>
+        <v>8.2175925925925923E-3</v>
       </c>
       <c r="G70" s="2">
         <v>3</v>
@@ -11069,22 +11071,22 @@
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="E71" s="1">
         <v>0</v>
       </c>
       <c r="F71" s="4">
-        <v>8.171296296296298E-3</v>
+        <v>8.2291666666666659E-3</v>
       </c>
       <c r="G71" s="2">
         <v>3</v>
@@ -11092,22 +11094,22 @@
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="E72" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F72" s="4">
-        <v>8.2175925925925923E-3</v>
+        <v>8.4722222222222213E-3</v>
       </c>
       <c r="G72" s="2">
         <v>3</v>
@@ -11115,10 +11117,10 @@
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>17</v>
@@ -11130,7 +11132,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="4">
-        <v>8.2291666666666659E-3</v>
+        <v>8.6111111111111145E-3</v>
       </c>
       <c r="G73" s="2">
         <v>3</v>
@@ -11138,68 +11140,68 @@
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E74" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74" s="4">
-        <v>8.4722222222222213E-3</v>
+        <v>8.9814814814814826E-3</v>
       </c>
       <c r="G74" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B75" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="E75" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F75" s="4">
-        <v>8.6111111111111145E-3</v>
+        <v>9.1666666666666667E-3</v>
       </c>
       <c r="G75" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B76" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E76" s="1">
         <v>2</v>
       </c>
       <c r="F76" s="4">
-        <v>8.9814814814814826E-3</v>
+        <v>9.3402777777777772E-3</v>
       </c>
       <c r="G76" s="2">
         <v>4</v>
@@ -11207,22 +11209,22 @@
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B77" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E77" s="1">
         <v>2</v>
       </c>
       <c r="F77" s="4">
-        <v>9.1666666666666667E-3</v>
+        <v>9.5138888888888877E-3</v>
       </c>
       <c r="G77" s="2">
         <v>4</v>
@@ -11230,10 +11232,10 @@
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B78" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>17</v>
@@ -11245,7 +11247,7 @@
         <v>2</v>
       </c>
       <c r="F78" s="4">
-        <v>9.3402777777777772E-3</v>
+        <v>9.5486111111111084E-3</v>
       </c>
       <c r="G78" s="2">
         <v>4</v>
@@ -11253,22 +11255,22 @@
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B79" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E79" s="1">
         <v>2</v>
       </c>
       <c r="F79" s="4">
-        <v>9.5138888888888877E-3</v>
+        <v>9.6874999999999982E-3</v>
       </c>
       <c r="G79" s="2">
         <v>4</v>
@@ -11276,10 +11278,10 @@
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B80" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>17</v>
@@ -11291,7 +11293,7 @@
         <v>2</v>
       </c>
       <c r="F80" s="4">
-        <v>9.5486111111111084E-3</v>
+        <v>9.7916666666666673E-3</v>
       </c>
       <c r="G80" s="2">
         <v>4</v>
@@ -11299,10 +11301,10 @@
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B81" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>17</v>
@@ -11314,7 +11316,7 @@
         <v>2</v>
       </c>
       <c r="F81" s="4">
-        <v>9.6874999999999982E-3</v>
+        <v>9.9421296296296306E-3</v>
       </c>
       <c r="G81" s="2">
         <v>4</v>
@@ -11322,10 +11324,10 @@
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B82" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>17</v>
@@ -11337,7 +11339,7 @@
         <v>2</v>
       </c>
       <c r="F82" s="4">
-        <v>9.7916666666666673E-3</v>
+        <v>1.0011574074074072E-2</v>
       </c>
       <c r="G82" s="2">
         <v>4</v>
@@ -11345,10 +11347,10 @@
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B83" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>17</v>
@@ -11360,7 +11362,7 @@
         <v>2</v>
       </c>
       <c r="F83" s="4">
-        <v>9.9421296296296306E-3</v>
+        <v>1.0069444444444447E-2</v>
       </c>
       <c r="G83" s="2">
         <v>4</v>
@@ -11368,10 +11370,10 @@
     </row>
     <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B84" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>17</v>
@@ -11380,56 +11382,56 @@
         <v>18</v>
       </c>
       <c r="E84" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" s="4">
-        <v>1.0011574074074072E-2</v>
+        <v>1.0335648148148146E-2</v>
       </c>
       <c r="G84" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B85" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E85" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F85" s="4">
-        <v>1.0069444444444447E-2</v>
+        <v>1.053240740740741E-2</v>
       </c>
       <c r="G85" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B86" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86" s="4">
-        <v>1.0335648148148146E-2</v>
+        <v>1.0763888888888889E-2</v>
       </c>
       <c r="G86" s="2">
         <v>5</v>
@@ -11437,22 +11439,22 @@
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B87" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E87" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87" s="4">
-        <v>1.053240740740741E-2</v>
+        <v>1.0879629629629631E-2</v>
       </c>
       <c r="G87" s="2">
         <v>5</v>
@@ -11460,13 +11462,13 @@
     </row>
     <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>32</v>
@@ -11475,7 +11477,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="4">
-        <v>1.0763888888888889E-2</v>
+        <v>1.1087962962962963E-2</v>
       </c>
       <c r="G88" s="2">
         <v>5</v>
@@ -11483,22 +11485,22 @@
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B89" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E89" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F89" s="4">
-        <v>1.0879629629629631E-2</v>
+        <v>1.1180555555555558E-2</v>
       </c>
       <c r="G89" s="2">
         <v>5</v>
@@ -11506,10 +11508,10 @@
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B90" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>17</v>
@@ -11521,7 +11523,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="4">
-        <v>1.1087962962962963E-2</v>
+        <v>1.1226851851851852E-2</v>
       </c>
       <c r="G90" s="2">
         <v>5</v>
@@ -11529,10 +11531,10 @@
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>17</v>
@@ -11544,7 +11546,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="4">
-        <v>1.1180555555555558E-2</v>
+        <v>1.1331018518518522E-2</v>
       </c>
       <c r="G91" s="2">
         <v>5</v>
@@ -11552,13 +11554,13 @@
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B92" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>32</v>
@@ -11567,7 +11569,7 @@
         <v>0</v>
       </c>
       <c r="F92" s="4">
-        <v>1.1226851851851852E-2</v>
+        <v>1.1481481481481485E-2</v>
       </c>
       <c r="G92" s="2">
         <v>5</v>
@@ -11575,22 +11577,22 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B93" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E93" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F93" s="4">
-        <v>1.1331018518518522E-2</v>
+        <v>1.1689814814814816E-2</v>
       </c>
       <c r="G93" s="2">
         <v>5</v>
@@ -11598,22 +11600,22 @@
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B94" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E94" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F94" s="4">
-        <v>1.1481481481481485E-2</v>
+        <v>1.2314814814814817E-2</v>
       </c>
       <c r="G94" s="2">
         <v>5</v>
@@ -11621,10 +11623,10 @@
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B95" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>17</v>
@@ -11636,7 +11638,7 @@
         <v>2</v>
       </c>
       <c r="F95" s="4">
-        <v>1.1689814814814816E-2</v>
+        <v>1.2592592592592596E-2</v>
       </c>
       <c r="G95" s="2">
         <v>5</v>
@@ -11644,22 +11646,22 @@
     </row>
     <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B96" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="E96" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F96" s="4">
-        <v>1.2314814814814817E-2</v>
+        <v>1.2708333333333332E-2</v>
       </c>
       <c r="G96" s="2">
         <v>5</v>
@@ -11667,10 +11669,10 @@
     </row>
     <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B97" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>17</v>
@@ -11679,10 +11681,10 @@
         <v>18</v>
       </c>
       <c r="E97" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" s="4">
-        <v>1.2592592592592596E-2</v>
+        <v>1.2870370370370369E-2</v>
       </c>
       <c r="G97" s="2">
         <v>5</v>
@@ -11690,22 +11692,22 @@
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B98" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="E98" s="1">
         <v>0</v>
       </c>
       <c r="F98" s="4">
-        <v>1.2708333333333332E-2</v>
+        <v>1.3171296296296296E-2</v>
       </c>
       <c r="G98" s="2">
         <v>5</v>
@@ -11713,13 +11715,13 @@
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B99" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>18</v>
@@ -11728,7 +11730,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="4">
-        <v>1.2870370370370369E-2</v>
+        <v>1.3252314814814817E-2</v>
       </c>
       <c r="G99" s="2">
         <v>5</v>
@@ -11736,22 +11738,22 @@
     </row>
     <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B100" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E100" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" s="4">
-        <v>1.3171296296296296E-2</v>
+        <v>1.3645833333333333E-2</v>
       </c>
       <c r="G100" s="2">
         <v>5</v>
@@ -11759,13 +11761,13 @@
     </row>
     <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B101" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>18</v>
@@ -11774,7 +11776,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="4">
-        <v>1.3252314814814817E-2</v>
+        <v>1.3831018518518517E-2</v>
       </c>
       <c r="G101" s="2">
         <v>5</v>
@@ -11782,10 +11784,10 @@
     </row>
     <row r="102" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B102" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>17</v>
@@ -11797,7 +11799,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="4">
-        <v>1.3645833333333333E-2</v>
+        <v>1.4039351851851855E-2</v>
       </c>
       <c r="G102" s="2">
         <v>5</v>
@@ -11805,10 +11807,10 @@
     </row>
     <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B103" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>17</v>
@@ -11817,10 +11819,10 @@
         <v>18</v>
       </c>
       <c r="E103" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F103" s="4">
-        <v>1.3831018518518517E-2</v>
+        <v>1.4166666666666664E-2</v>
       </c>
       <c r="G103" s="2">
         <v>5</v>
@@ -11828,10 +11830,10 @@
     </row>
     <row r="104" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B104" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>17</v>
@@ -11840,10 +11842,10 @@
         <v>18</v>
       </c>
       <c r="E104" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F104" s="4">
-        <v>1.4039351851851855E-2</v>
+        <v>1.425925925925926E-2</v>
       </c>
       <c r="G104" s="2">
         <v>5</v>
@@ -11851,22 +11853,22 @@
     </row>
     <row r="105" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B105" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E105" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F105" s="4">
-        <v>1.4166666666666664E-2</v>
+        <v>1.443287037037037E-2</v>
       </c>
       <c r="G105" s="2">
         <v>5</v>
@@ -11874,22 +11876,22 @@
     </row>
     <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B106" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E106" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F106" s="4">
-        <v>1.425925925925926E-2</v>
+        <v>1.4513888888888892E-2</v>
       </c>
       <c r="G106" s="2">
         <v>5</v>
@@ -11897,22 +11899,22 @@
     </row>
     <row r="107" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B107" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="E107" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" s="4">
-        <v>1.443287037037037E-2</v>
+        <v>1.4606481481481481E-2</v>
       </c>
       <c r="G107" s="2">
         <v>5</v>
@@ -11920,22 +11922,22 @@
     </row>
     <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B108" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="E108" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" s="4">
-        <v>1.4513888888888892E-2</v>
+        <v>1.4930555555555555E-2</v>
       </c>
       <c r="G108" s="2">
         <v>5</v>
@@ -11943,10 +11945,10 @@
     </row>
     <row r="109" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B109" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>17</v>
@@ -11955,10 +11957,10 @@
         <v>18</v>
       </c>
       <c r="E109" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F109" s="4">
-        <v>1.4606481481481481E-2</v>
+        <v>1.4976851851851856E-2</v>
       </c>
       <c r="G109" s="2">
         <v>5</v>
@@ -11966,10 +11968,10 @@
     </row>
     <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B110" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>17</v>
@@ -11978,10 +11980,10 @@
         <v>18</v>
       </c>
       <c r="E110" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F110" s="4">
-        <v>1.4930555555555555E-2</v>
+        <v>1.5196759259259261E-2</v>
       </c>
       <c r="G110" s="2">
         <v>5</v>
@@ -11989,10 +11991,10 @@
     </row>
     <row r="111" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B111" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>17</v>
@@ -12001,10 +12003,10 @@
         <v>18</v>
       </c>
       <c r="E111" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F111" s="4">
-        <v>1.4976851851851856E-2</v>
+        <v>1.5358796296296297E-2</v>
       </c>
       <c r="G111" s="2">
         <v>5</v>
@@ -12012,10 +12014,10 @@
     </row>
     <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B112" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>17</v>
@@ -12027,7 +12029,7 @@
         <v>2</v>
       </c>
       <c r="F112" s="4">
-        <v>1.5196759259259261E-2</v>
+        <v>1.5509259259259261E-2</v>
       </c>
       <c r="G112" s="2">
         <v>5</v>
@@ -12035,10 +12037,10 @@
     </row>
     <row r="113" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B113" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>17</v>
@@ -12050,7 +12052,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="4">
-        <v>1.5358796296296297E-2</v>
+        <v>1.5648148148148151E-2</v>
       </c>
       <c r="G113" s="2">
         <v>5</v>
@@ -12058,10 +12060,10 @@
     </row>
     <row r="114" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B114" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>17</v>
@@ -12070,10 +12072,10 @@
         <v>18</v>
       </c>
       <c r="E114" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F114" s="4">
-        <v>1.5509259259259261E-2</v>
+        <v>1.6064814814814813E-2</v>
       </c>
       <c r="G114" s="2">
         <v>5</v>
@@ -12081,10 +12083,10 @@
     </row>
     <row r="115" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B115" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>17</v>
@@ -12093,10 +12095,10 @@
         <v>18</v>
       </c>
       <c r="E115" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F115" s="4">
-        <v>1.5648148148148151E-2</v>
+        <v>1.6180555555555556E-2</v>
       </c>
       <c r="G115" s="2">
         <v>5</v>
@@ -12104,10 +12106,10 @@
     </row>
     <row r="116" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B116" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>17</v>
@@ -12119,7 +12121,7 @@
         <v>1</v>
       </c>
       <c r="F116" s="4">
-        <v>1.6064814814814813E-2</v>
+        <v>1.6331018518518519E-2</v>
       </c>
       <c r="G116" s="2">
         <v>5</v>
@@ -12127,10 +12129,10 @@
     </row>
     <row r="117" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B117" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>17</v>
@@ -12142,7 +12144,7 @@
         <v>2</v>
       </c>
       <c r="F117" s="4">
-        <v>1.6180555555555556E-2</v>
+        <v>1.6631944444444446E-2</v>
       </c>
       <c r="G117" s="2">
         <v>5</v>
@@ -12150,10 +12152,10 @@
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B118" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>17</v>
@@ -12162,10 +12164,10 @@
         <v>18</v>
       </c>
       <c r="E118" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F118" s="4">
-        <v>1.6331018518518519E-2</v>
+        <v>1.681712962962963E-2</v>
       </c>
       <c r="G118" s="2">
         <v>5</v>
@@ -12173,10 +12175,10 @@
     </row>
     <row r="119" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B119" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>17</v>
@@ -12188,7 +12190,7 @@
         <v>2</v>
       </c>
       <c r="F119" s="4">
-        <v>1.6631944444444446E-2</v>
+        <v>1.7037037037037035E-2</v>
       </c>
       <c r="G119" s="2">
         <v>5</v>
@@ -12196,10 +12198,10 @@
     </row>
     <row r="120" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B120" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>17</v>
@@ -12211,58 +12213,14 @@
         <v>2</v>
       </c>
       <c r="F120" s="4">
-        <v>1.681712962962963E-2</v>
+        <v>1.7118055555555556E-2</v>
       </c>
       <c r="G120" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B121" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E121" s="1">
-        <v>2</v>
-      </c>
-      <c r="F121" s="4">
-        <v>1.7037037037037035E-2</v>
-      </c>
-      <c r="G121" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B122" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E122" s="1">
-        <v>2</v>
-      </c>
-      <c r="F122" s="4">
-        <v>1.7118055555555556E-2</v>
-      </c>
-      <c r="G122" s="2">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="121" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="123" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="124" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="125" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13139,8 +13097,6 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>